<commit_message>
add fileds and modify the form
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,101 +1,218 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dispensaire-my.sharepoint.com/personal/ldridi_dispensaire_ca/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nader\Documents\projets_lotfi\App-laptops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{EA5BB46D-E0E8-4B35-BC98-958A81D6BA90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{2067603F-9348-4C79-8ACB-757CFD85221A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86DB160-BD47-4EE7-B0C3-45D2CDC7AE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
   <si>
+    <t>Nom de l'appareil</t>
+  </si>
+  <si>
+    <t>Marque</t>
+  </si>
+  <si>
+    <t>Date de l'achat</t>
+  </si>
+  <si>
+    <t>Form Number</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Email id</t>
+  </si>
+  <si>
+    <t>Amortissement mensuel</t>
+  </si>
+  <si>
+    <t>Dotation aux amortissements</t>
+  </si>
+  <si>
+    <t>Valeure compatable nette</t>
+  </si>
+  <si>
+    <t>Utilisateur</t>
+  </si>
+  <si>
+    <t>Date affectation</t>
+  </si>
+  <si>
     <t>DDM-PF3A47NZ</t>
   </si>
   <si>
+    <t>Laptop-LENOVO</t>
+  </si>
+  <si>
+    <t>G2*nombre de mois écoulés de puis la date d'achat</t>
+  </si>
+  <si>
+    <t>McCarthy, Andrea</t>
+  </si>
+  <si>
+    <t>jj/mm/aaaa</t>
+  </si>
+  <si>
     <t>DDM-PF2E6RFJ</t>
   </si>
   <si>
+    <t>Zeggane, Ouardia</t>
+  </si>
+  <si>
     <t>DDM-PF3MS2HF</t>
   </si>
   <si>
+    <t>Tran, Cam-Tam</t>
+  </si>
+  <si>
     <t>DDM-PF1GWV8B</t>
   </si>
   <si>
+    <t>Fréchette-Doyon, Lorrance</t>
+  </si>
+  <si>
     <t>DDM-PF3MS2J7</t>
   </si>
   <si>
+    <t>Vézina, Catherine</t>
+  </si>
+  <si>
     <t>DDM-PF2DXHZS</t>
   </si>
   <si>
+    <t>Lepage, Suzanne</t>
+  </si>
+  <si>
     <t>DDM-PF13HV5C</t>
   </si>
   <si>
+    <t>Guévin, Maude</t>
+  </si>
+  <si>
     <t>DDM-PF33TEAG</t>
   </si>
   <si>
+    <t>Gadoua, Alessia</t>
+  </si>
+  <si>
     <t>DDM-PF32MZ5E</t>
   </si>
   <si>
+    <t>Paquette, Julie</t>
+  </si>
+  <si>
     <t>DDM-PF1GW73L</t>
   </si>
   <si>
+    <t>Medeiros, Karen</t>
+  </si>
+  <si>
     <t>DDM-PF392830</t>
   </si>
   <si>
+    <t>Dridi, Lotfi</t>
+  </si>
+  <si>
     <t>DDM-PF32MZ5X</t>
   </si>
   <si>
+    <t>MEKHOUKH, ZOÉ</t>
+  </si>
+  <si>
     <t>DDM-PF1GWV85</t>
   </si>
   <si>
+    <t>Buckett, Selma</t>
+  </si>
+  <si>
     <t>DDM-PF4967L1</t>
   </si>
   <si>
+    <t>Delorme, Julie</t>
+  </si>
+  <si>
     <t>DDM-PF32W0FS</t>
   </si>
   <si>
+    <t>Borgatta, Olivia</t>
+  </si>
+  <si>
     <t>DDM-PF33TF28</t>
   </si>
   <si>
+    <t>Hiriart Madrazo, Maria De Lourdes</t>
+  </si>
+  <si>
     <t>DDM-PF2ACSD5</t>
   </si>
   <si>
+    <t>Proulx-Alonzo, France</t>
+  </si>
+  <si>
     <t>DDM-PF2E6X11</t>
   </si>
   <si>
+    <t>gc2m</t>
+  </si>
+  <si>
     <t>DDM-PF12T1YQ</t>
   </si>
   <si>
+    <t>Boulad, Maryam</t>
+  </si>
+  <si>
     <t>DDM-PF3A47L6</t>
   </si>
   <si>
+    <t>Tremblay, Stéphanie</t>
+  </si>
+  <si>
     <t>DDM-PF13HSZ1</t>
   </si>
   <si>
+    <t>Royer, Catherine</t>
+  </si>
+  <si>
     <t>DDM-PF1GWV75</t>
   </si>
   <si>
+    <t>Labelle, Catherine</t>
+  </si>
+  <si>
     <t>DDM-DC01</t>
   </si>
   <si>
     <t>Server</t>
   </si>
   <si>
-    <t>gc2m</t>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>aaaa-mm-jj</t>
+  </si>
+  <si>
+    <t>Salonina, Dina</t>
+  </si>
+  <si>
+    <t>Le prix est donné a titre indicatif</t>
   </si>
   <si>
     <t>Employés (1 - 23)</t>
@@ -128,154 +245,37 @@
     <t>Compagnie</t>
   </si>
   <si>
-    <t>Borgatta, Olivia</t>
-  </si>
-  <si>
     <t>70-702</t>
   </si>
   <si>
     <t>Actif</t>
   </si>
   <si>
-    <t>Boulad, Maryam</t>
-  </si>
-  <si>
     <t>50-501</t>
   </si>
   <si>
-    <t>Buckett, Selma</t>
-  </si>
-  <si>
     <t>50-502</t>
   </si>
   <si>
-    <t>Delorme, Julie</t>
-  </si>
-  <si>
     <t>90-902</t>
   </si>
   <si>
-    <t>Dridi, Lotfi</t>
-  </si>
-  <si>
     <t>70-700</t>
   </si>
   <si>
-    <t>Fréchette-Doyon, Lorrance</t>
-  </si>
-  <si>
     <t>50-503</t>
   </si>
   <si>
-    <t>Gadoua, Alessia</t>
-  </si>
-  <si>
-    <t>Guévin, Maude</t>
-  </si>
-  <si>
-    <t>Hiriart Madrazo, Maria De Lourdes</t>
-  </si>
-  <si>
     <t>Houle, Alexia</t>
   </si>
   <si>
-    <t>Labelle, Catherine</t>
-  </si>
-  <si>
-    <t>Lepage, Suzanne</t>
-  </si>
-  <si>
     <t>70-701</t>
   </si>
   <si>
-    <t>McCarthy, Andrea</t>
-  </si>
-  <si>
-    <t>Medeiros, Karen</t>
-  </si>
-  <si>
-    <t>MEKHOUKH, ZOÉ</t>
-  </si>
-  <si>
-    <t>Paquette, Julie</t>
-  </si>
-  <si>
-    <t>Proulx-Alonzo, France</t>
-  </si>
-  <si>
-    <t>Royer, Catherine</t>
-  </si>
-  <si>
-    <t>Salonina, Dina</t>
-  </si>
-  <si>
-    <t>Tran, Cam-Tam</t>
-  </si>
-  <si>
     <t>10-001</t>
   </si>
   <si>
-    <t>Tremblay, Stéphanie</t>
-  </si>
-  <si>
-    <t>Vézina, Catherine</t>
-  </si>
-  <si>
     <t>90-900</t>
-  </si>
-  <si>
-    <t>Zeggane, Ouardia</t>
-  </si>
-  <si>
-    <t>Nom de l'appareil</t>
-  </si>
-  <si>
-    <t>Utilisateur</t>
-  </si>
-  <si>
-    <t>Laptop-LENOVO</t>
-  </si>
-  <si>
-    <t>Marque</t>
-  </si>
-  <si>
-    <t>Date d’achat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prix d'achat </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date affectation </t>
-  </si>
-  <si>
-    <t>jj/mm/aaaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date comptabilisation </t>
-  </si>
-  <si>
-    <t>Amortissement mensuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date d'éxpiration </t>
-  </si>
-  <si>
-    <t>Le prix est donné a titre indicatif</t>
-  </si>
-  <si>
-    <t>Dotation aux amortissements</t>
-  </si>
-  <si>
-    <t>Valeure compatable nette</t>
-  </si>
-  <si>
-    <t>G2*nombre de mois écoulés de puis la date d'achat</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>aaaa-mm-jj</t>
   </si>
 </sst>
 </file>
@@ -283,9 +283,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;_);[Red]\(#,##0\ &quot;$&quot;\)"/>
     <numFmt numFmtId="164" formatCode="*@"/>
-    <numFmt numFmtId="170" formatCode="yyyy/mm"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm"/>
+    <numFmt numFmtId="166" formatCode="#,##0\ &quot;$&quot;_);[Red]\(#,##0\ &quot;$&quot;\)"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -324,19 +324,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="30" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,683 +652,683 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.44140625" customWidth="1"/>
-    <col min="10" max="10" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="50" customWidth="1"/>
+    <col min="8" max="8" width="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50" customWidth="1"/>
+    <col min="10" max="11" width="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>74</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1">
         <v>44692</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>45787</v>
       </c>
       <c r="E2" s="7">
         <v>1111</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="8">
         <v>45787</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="4">
         <f>E2*0.3/12</f>
         <v>27.775000000000002</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="I2" s="8" t="e">
-        <f xml:space="preserve"> G2-H2</f>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="e">
+        <f>G2-H2</f>
         <v>#VALUE!</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>75</v>
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
         <v>44068</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>45162</v>
       </c>
       <c r="E3" s="7">
         <v>1112</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="8">
         <v>45162</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <f>E3*0.3/12</f>
         <v>27.799999999999997</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
         <v>44754</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>45849</v>
       </c>
       <c r="E4" s="7">
         <v>1113</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="8">
         <v>45849</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
         <v>43530</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>44625</v>
       </c>
       <c r="E5" s="7">
         <v>1114</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="8">
         <v>44625</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
         <v>44754</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>45849</v>
       </c>
       <c r="E6" s="7">
         <v>1115</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="8">
         <v>45849</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
         <v>44068</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>45162</v>
       </c>
       <c r="E7" s="7">
         <v>1116</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="8">
         <v>45162</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
         <v>43759</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>44854</v>
       </c>
       <c r="E8" s="7">
         <v>1117</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="8">
         <v>44854</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
         <v>44561</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>45656</v>
       </c>
       <c r="E9" s="7">
         <v>1118</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="8">
         <v>45656</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
         <v>44468</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>45563</v>
       </c>
       <c r="E10" s="7">
         <v>1119</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="8">
         <v>45563</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="A11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1">
         <v>43529</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>44624</v>
       </c>
       <c r="E11" s="7">
         <v>1120</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="8">
         <v>44624</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1">
         <v>44553</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>45648</v>
       </c>
       <c r="E12" s="7">
         <v>1121</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="8">
         <v>45648</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
         <v>44460</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>45555</v>
       </c>
       <c r="E13" s="7">
         <v>1122</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="8">
         <v>45555</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1">
         <v>43529</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>44624</v>
       </c>
       <c r="E14" s="7">
         <v>1123</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="8">
         <v>44624</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
       <c r="J14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
         <v>45002</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>46097</v>
       </c>
       <c r="E15" s="7">
         <v>1124</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="8">
         <v>46097</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
         <v>44460</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>45555</v>
       </c>
       <c r="E16" s="7">
         <v>1125</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="8">
         <v>45555</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="A17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
         <v>44595</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>45690</v>
       </c>
       <c r="E17" s="7">
         <v>1126</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="8">
         <v>45690</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
       <c r="J17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="A18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
         <v>44068</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>45162</v>
       </c>
       <c r="E18" s="7">
         <v>1127</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="8">
         <v>45162</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
       <c r="J18" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="A19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
         <v>44068</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>45162</v>
       </c>
       <c r="E19" s="7">
         <v>1128</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="8">
         <v>45162</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="1" t="s">
-        <v>24</v>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="A20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1">
         <v>43223</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>44318</v>
       </c>
       <c r="E20" s="7">
         <v>1129</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="8">
         <v>44318</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
       <c r="J20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="A21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
         <v>44692</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>45787</v>
       </c>
       <c r="E21" s="7">
         <v>1130</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="8">
         <v>45787</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="A22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1">
         <v>43759</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>44854</v>
       </c>
       <c r="E22" s="7">
         <v>1131</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="8">
         <v>44854</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
       <c r="J22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="A23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1">
         <v>43529</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>44624</v>
       </c>
       <c r="E23" s="7">
         <v>1132</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="8">
         <v>44624</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
       <c r="J23" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="A24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1">
         <v>44187</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>46014</v>
       </c>
       <c r="E24" s="7">
         <v>1133</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="8">
         <v>46014</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="B25" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>84</v>
+      <c r="B25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="J25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="E26" s="3" t="s">
-        <v>79</v>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1339,50 +1338,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFEF64C-3711-429F-AD1E-B1CFB86467C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D5:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:12">
       <c r="D5" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="4:12">
       <c r="D7" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="4:12">
@@ -1390,10 +1389,10 @@
         <v>97979</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="G8">
         <v>70</v>
@@ -1408,7 +1407,7 @@
         <v>999</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L8">
         <v>231438</v>
@@ -1419,10 +1418,10 @@
         <v>97991</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G9">
         <v>50</v>
@@ -1437,7 +1436,7 @@
         <v>999</v>
       </c>
       <c r="K9" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L9">
         <v>231438</v>
@@ -1448,10 +1447,10 @@
         <v>23150</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="G10">
         <v>50</v>
@@ -1466,7 +1465,7 @@
         <v>999</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L10">
         <v>231438</v>
@@ -1477,10 +1476,10 @@
         <v>97993</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="G11">
         <v>90</v>
@@ -1495,7 +1494,7 @@
         <v>999</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L11">
         <v>231438</v>
@@ -1506,10 +1505,10 @@
         <v>97975</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G12">
         <v>70</v>
@@ -1524,7 +1523,7 @@
         <v>999</v>
       </c>
       <c r="K12" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L12">
         <v>231438</v>
@@ -1535,10 +1534,10 @@
         <v>49726</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="G13">
         <v>50</v>
@@ -1553,7 +1552,7 @@
         <v>999</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L13">
         <v>231438</v>
@@ -1564,10 +1563,10 @@
         <v>97984</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="G14">
         <v>90</v>
@@ -1582,7 +1581,7 @@
         <v>999</v>
       </c>
       <c r="K14" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L14">
         <v>231438</v>
@@ -1593,10 +1592,10 @@
         <v>97983</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G15">
         <v>50</v>
@@ -1611,7 +1610,7 @@
         <v>999</v>
       </c>
       <c r="K15" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L15">
         <v>231438</v>
@@ -1622,7 +1621,7 @@
         <v>97990</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F16">
         <v>500</v>
@@ -1640,7 +1639,7 @@
         <v>999</v>
       </c>
       <c r="K16" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L16">
         <v>231438</v>
@@ -1651,10 +1650,10 @@
         <v>97992</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G17">
         <v>50</v>
@@ -1669,7 +1668,7 @@
         <v>999</v>
       </c>
       <c r="K17" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L17">
         <v>231438</v>
@@ -1680,10 +1679,10 @@
         <v>58500</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G18">
         <v>50</v>
@@ -1698,7 +1697,7 @@
         <v>999</v>
       </c>
       <c r="K18" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L18">
         <v>231438</v>
@@ -1709,10 +1708,10 @@
         <v>60528</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G19">
         <v>70</v>
@@ -1727,7 +1726,7 @@
         <v>999</v>
       </c>
       <c r="K19" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L19">
         <v>231438</v>
@@ -1738,10 +1737,10 @@
         <v>76131</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G20">
         <v>50</v>
@@ -1756,7 +1755,7 @@
         <v>999</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L20">
         <v>231438</v>
@@ -1767,10 +1766,10 @@
         <v>80550</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G21">
         <v>50</v>
@@ -1785,7 +1784,7 @@
         <v>999</v>
       </c>
       <c r="K21" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L21">
         <v>231438</v>
@@ -1796,10 +1795,10 @@
         <v>97982</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G22">
         <v>10</v>
@@ -1814,7 +1813,7 @@
         <v>999</v>
       </c>
       <c r="K22" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L22">
         <v>231438</v>
@@ -1825,10 +1824,10 @@
         <v>97978</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G23">
         <v>70</v>
@@ -1843,7 +1842,7 @@
         <v>999</v>
       </c>
       <c r="K23" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L23">
         <v>231438</v>
@@ -1854,10 +1853,10 @@
         <v>92924</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G24">
         <v>50</v>
@@ -1872,7 +1871,7 @@
         <v>999</v>
       </c>
       <c r="K24" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L24">
         <v>231438</v>
@@ -1883,10 +1882,10 @@
         <v>97988</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G25">
         <v>50</v>
@@ -1901,7 +1900,7 @@
         <v>999</v>
       </c>
       <c r="K25" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L25">
         <v>231438</v>
@@ -1912,10 +1911,10 @@
         <v>93477</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G26">
         <v>50</v>
@@ -1930,7 +1929,7 @@
         <v>999</v>
       </c>
       <c r="K26" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L26">
         <v>231438</v>
@@ -1941,10 +1940,10 @@
         <v>81850</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G27">
         <v>10</v>
@@ -1959,7 +1958,7 @@
         <v>999</v>
       </c>
       <c r="K27" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L27">
         <v>231438</v>
@@ -1970,10 +1969,10 @@
         <v>97986</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G28">
         <v>70</v>
@@ -1988,7 +1987,7 @@
         <v>999</v>
       </c>
       <c r="K28" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L28">
         <v>231438</v>
@@ -1999,10 +1998,10 @@
         <v>97971</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G29">
         <v>90</v>
@@ -2017,7 +2016,7 @@
         <v>999</v>
       </c>
       <c r="K29" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="L29">
         <v>231438</v>
@@ -2028,10 +2027,10 @@
         <v>97968</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G30">
         <v>50</v>
@@ -2046,299 +2045,11 @@
         <v>999</v>
       </c>
       <c r="K30" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058581DBD2DEFEF47B5C706E38806CDB6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2b7394842d1f32ff509e27291f21df5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e648cdfb-1b41-45ea-85c2-239838855cb4" xmlns:ns4="aef4cc67-8959-445d-8e07-f989da035ba0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc63d34ecdd03d3198f52ad119a103c7" ns3:_="" ns4:_="">
-    <xsd:import namespace="e648cdfb-1b41-45ea-85c2-239838855cb4"/>
-    <xsd:import namespace="aef4cc67-8959-445d-8e07-f989da035ba0"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns4:_activity" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e648cdfb-1b41-45ea-85c2-239838855cb4" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="aef4cc67-8959-445d-8e07-f989da035ba0" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="_activity" ma:index="20" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="aef4cc67-8959-445d-8e07-f989da035ba0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{512A6283-959B-4B5E-ABF9-AC2356A2EE47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e648cdfb-1b41-45ea-85c2-239838855cb4"/>
-    <ds:schemaRef ds:uri="aef4cc67-8959-445d-8e07-f989da035ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E2AC2C2-B3FB-4633-A498-C2E187FD1008}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{045CB323-30B6-4EE7-9F1F-302267CA15B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="aef4cc67-8959-445d-8e07-f989da035ba0"/>
-    <ds:schemaRef ds:uri="e648cdfb-1b41-45ea-85c2-239838855cb4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>